<commit_message>
enable download of student progress report as csv and reverse order of notes
</commit_message>
<xml_diff>
--- a/data/facultyTemp.xlsx
+++ b/data/facultyTemp.xlsx
@@ -375,72 +375,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>pronouns</v>
+      </c>
+      <c r="B1" t="str">
+        <v>status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>gender</v>
+      </c>
+      <c r="D1" t="str">
+        <v>ethnicity</v>
+      </c>
+      <c r="E1" t="str">
+        <v>residency</v>
+      </c>
+      <c r="F1" t="str">
+        <v>intendedDegree</v>
+      </c>
+      <c r="G1" t="str">
+        <v>fundingEligibility</v>
+      </c>
+      <c r="H1" t="str">
+        <v>jobHistory</v>
+      </c>
+      <c r="I1" t="str">
+        <v>grades</v>
+      </c>
+      <c r="J1" t="str">
         <v>onyen</v>
       </c>
-      <c r="B1" t="str">
+      <c r="K1" t="str">
         <v>csid</v>
       </c>
-      <c r="C1" t="str">
+      <c r="L1" t="str">
         <v>email</v>
       </c>
-      <c r="D1" t="str">
+      <c r="M1" t="str">
         <v>firstName</v>
       </c>
-      <c r="E1" t="str">
+      <c r="N1" t="str">
         <v>lastName</v>
       </c>
-      <c r="F1" t="str">
+      <c r="O1" t="str">
         <v>pid</v>
       </c>
-      <c r="G1" t="str">
-        <v>sectionNumber</v>
-      </c>
-      <c r="H1" t="str">
-        <v>active</v>
-      </c>
-      <c r="I1" t="str">
-        <v>admin</v>
+      <c r="P1" t="str">
+        <v>citizenship</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>advisor</v>
+      </c>
+      <c r="R1" t="str">
+        <v>researchAdvisor</v>
+      </c>
+      <c r="S1" t="str">
+        <v>prpPassed</v>
+      </c>
+      <c r="T1" t="str">
+        <v>phdAwarded</v>
+      </c>
+      <c r="U1" t="str">
+        <v>dissertationSubmitted</v>
+      </c>
+      <c r="V1" t="str">
+        <v>semestersOnLeave</v>
+      </c>
+      <c r="W1" t="str">
+        <v>hoursCompleted</v>
+      </c>
+      <c r="X1" t="str">
+        <v>alternativeName</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>enteringStatus</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>researchArea</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>leaveExtension</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>backgroundApproved</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>mastersAwarded</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>technicalWritingApproved</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>backgroundPrepWorksheetApproved</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>programOfStudyApproved</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>researchPlanningMeeting</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>programProductRequirement</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>committeeCompApproved</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>phdProposalApproved</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>oralExamPassed</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>dissertationDefencePassed</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>semesterStarted</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>proceedToPhdFormSubmitted</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>otherAdvisor</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>otherResearchAdvisor</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>person</v>
+        <v>None</v>
       </c>
       <c r="B2" t="str">
-        <v>person</v>
+        <v>Active</v>
       </c>
       <c r="C2" t="str">
-        <v>varuntanna23@gmail.com</v>
+        <v>OTHER</v>
       </c>
       <c r="D2" t="str">
-        <v>person</v>
+        <v>OTHER</v>
       </c>
       <c r="E2" t="str">
-        <v>person</v>
-      </c>
-      <c r="F2">
+        <v>YES</v>
+      </c>
+      <c r="F2" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G2" t="str">
+        <v>NOT GUARANTEED</v>
+      </c>
+      <c r="J2" t="str">
+        <v>testcreate</v>
+      </c>
+      <c r="K2" t="str">
+        <v>testcreate</v>
+      </c>
+      <c r="L2" t="str">
+        <v>testcreate@gmail.com</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Test</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Create</v>
+      </c>
+      <c r="O2">
+        <v>777777777</v>
+      </c>
+      <c r="P2" t="b">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="S2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>None</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Graduated</v>
+      </c>
+      <c r="C3" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="D3" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="E3" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F3" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G3" t="str">
+        <v>PROBATION</v>
+      </c>
+      <c r="J3" t="str">
+        <v>hmbodnar</v>
+      </c>
+      <c r="K3" t="str">
+        <v>iddd</v>
+      </c>
+      <c r="L3" t="str">
+        <v>hannahbodnar.17+student@gmail.com</v>
+      </c>
+      <c r="M3" t="str">
+        <v>hannah</v>
+      </c>
+      <c r="N3" t="str">
+        <v>bodnar</v>
+      </c>
+      <c r="O3">
+        <v>730171699</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="str">
+        <v/>
+      </c>
+      <c r="U3" t="str">
+        <v/>
+      </c>
+      <c r="W3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>she, her</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Graduated</v>
+      </c>
+      <c r="C4" t="str">
+        <v>FEMALE</v>
+      </c>
+      <c r="D4" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="E4" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F4" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G4" t="str">
+        <v>GUARANTEED</v>
+      </c>
+      <c r="J4" t="str">
+        <v>fakeonyen</v>
+      </c>
+      <c r="K4" t="str">
+        <v>fakecsid</v>
+      </c>
+      <c r="L4" t="str">
+        <v>fakeEmail@fake.com</v>
+      </c>
+      <c r="M4" t="str">
+        <v>fake</v>
+      </c>
+      <c r="N4" t="str">
+        <v>fake</v>
+      </c>
+      <c r="O4">
+        <v>949949949</v>
+      </c>
+      <c r="P4" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="b">
+      <c r="S4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="T4" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="U4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="V4">
+        <v>99</v>
+      </c>
+      <c r="W4">
+        <v>20</v>
+      </c>
+      <c r="X4" t="str">
+        <v>fake</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>help</v>
+      </c>
+      <c r="Z4" t="str">
+        <v>Systems</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>NO</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AC4" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="AD4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AF4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AG4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AH4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AI4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AJ4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AK4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AL4" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AN4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>she, her</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Graduated</v>
+      </c>
+      <c r="C5" t="str">
+        <v>FEMALE</v>
+      </c>
+      <c r="D5" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="E5" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F5" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G5" t="str">
+        <v>GUARANTEED</v>
+      </c>
+      <c r="J5" t="str">
+        <v>progress</v>
+      </c>
+      <c r="K5" t="str">
+        <v>progress</v>
+      </c>
+      <c r="L5" t="str">
+        <v>progress@gmail.com</v>
+      </c>
+      <c r="M5" t="str">
+        <v>progress</v>
+      </c>
+      <c r="N5" t="str">
+        <v>report</v>
+      </c>
+      <c r="O5">
+        <v>222222222</v>
+      </c>
+      <c r="P5" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="b">
+      <c r="S5" t="str">
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="U5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="V5">
         <v>1</v>
+      </c>
+      <c r="W5">
+        <v>20</v>
+      </c>
+      <c r="X5" t="str">
+        <v>fake</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>help</v>
+      </c>
+      <c r="Z5" t="str">
+        <v>Systems</v>
+      </c>
+      <c r="AA5" t="str">
+        <v>NO</v>
+      </c>
+      <c r="AB5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AC5" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="AD5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AE5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AF5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AG5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AH5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AI5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AJ5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AK5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AL5" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AN5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>None</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Active</v>
+      </c>
+      <c r="C6" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="D6" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="E6" t="str">
+        <v>NO</v>
+      </c>
+      <c r="F6" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NOT GUARANTEED</v>
+      </c>
+      <c r="J6" t="str">
+        <v>new</v>
+      </c>
+      <c r="K6" t="str">
+        <v>newnew</v>
+      </c>
+      <c r="L6" t="str">
+        <v>new@gmail.com</v>
+      </c>
+      <c r="M6" t="str">
+        <v>new</v>
+      </c>
+      <c r="N6" t="str">
+        <v>student</v>
+      </c>
+      <c r="O6">
+        <v>111111111</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="str">
+        <v/>
+      </c>
+      <c r="AP6" t="str">
+        <v>member, other</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>she, her</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Graduated</v>
+      </c>
+      <c r="C7" t="str">
+        <v>FEMALE</v>
+      </c>
+      <c r="D7" t="str">
+        <v>OTHER</v>
+      </c>
+      <c r="E7" t="str">
+        <v>YES</v>
+      </c>
+      <c r="F7" t="str">
+        <v>MASTERS</v>
+      </c>
+      <c r="G7" t="str">
+        <v>GUARANTEED</v>
+      </c>
+      <c r="J7" t="str">
+        <v>fake</v>
+      </c>
+      <c r="K7" t="str">
+        <v>fake</v>
+      </c>
+      <c r="L7" t="str">
+        <v>fake@gmail.com</v>
+      </c>
+      <c r="M7" t="str">
+        <v>test</v>
+      </c>
+      <c r="N7" t="str">
+        <v>upload</v>
+      </c>
+      <c r="O7">
+        <v>2828282</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="T7" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="U7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="V7">
+        <v>99</v>
+      </c>
+      <c r="W7">
+        <v>20</v>
+      </c>
+      <c r="X7" t="str">
+        <v>fake</v>
+      </c>
+      <c r="Y7" t="str">
+        <v>help</v>
+      </c>
+      <c r="Z7" t="str">
+        <v>Systems</v>
+      </c>
+      <c r="AA7" t="str">
+        <v>NO</v>
+      </c>
+      <c r="AB7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AC7" t="str">
+        <v>2019-02-01</v>
+      </c>
+      <c r="AD7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AE7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AF7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AG7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AH7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AI7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AJ7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AK7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AL7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="AN7" t="str">
+        <v/>
+      </c>
+      <c r="AO7" t="str">
+        <v>test, test</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AP7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>